<commit_message>
Se agrego titulos a las tablas del .xlsx
</commit_message>
<xml_diff>
--- a/IIB/CubicSplines_Proyect/Datos MetNum IIB.xlsx
+++ b/IIB/CubicSplines_Proyect/Datos MetNum IIB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naran\OneDrive\Escritorio\Quinto Semestre\Metodos Numericos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MetodosNumericos\IIB\CubicSplines_Proyect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6ABE8B-B510-4477-9E6F-53C1176CFD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC32142-39CF-495C-BCBC-6C19A571D5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EF4F8CD1-F150-4AF9-A780-971277984D68}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{EF4F8CD1-F150-4AF9-A780-971277984D68}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>S20</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Galerkin</t>
+  </si>
+  <si>
+    <t>S_20</t>
   </si>
 </sst>
 </file>
@@ -89,10 +95,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,21 +177,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,19 +521,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF32FFD3-2F8B-4F81-BD39-F4872F63453A}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="10" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="10" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -508,855 +543,877 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I2">
         <v>2.33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F3" s="4" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I3">
         <v>11.8</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="18" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="I5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.79</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>2.68</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>5.83</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>6.7</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f>(C7*1)/$I$3</f>
         <v>6.6949152542372881E-2</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f>(D7*1)/$I$2</f>
         <v>1.07725321888412</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>(E7*1)/$I$2</f>
         <v>1.150214592274678</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f>(F7*1)/$I$2</f>
         <v>2.5021459227467813</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <f>(G7*1)/$I$2</f>
         <v>2.8755364806866952</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2.6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>2.82</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>3.1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>6.71</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>7.78</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>2</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <f t="shared" ref="J8:J16" si="0">(C8*1)/$I$3</f>
         <v>0.22033898305084745</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f t="shared" ref="K8:K16" si="1">(D8*1)/$I$2</f>
         <v>1.2103004291845492</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <f t="shared" ref="L8:L16" si="2">(E8*1)/$I$2</f>
         <v>1.3304721030042919</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <f t="shared" ref="M8:M16" si="3">(F8*1)/$I$2</f>
         <v>2.8798283261802573</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <f t="shared" ref="N8:N16" si="4">(G8*1)/$I$2</f>
         <v>3.3390557939914163</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>4.3099999999999996</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>2.76</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2.98</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>6.68</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>7.7</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>3</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <f t="shared" si="0"/>
         <v>0.36525423728813555</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f t="shared" si="1"/>
         <v>1.1845493562231759</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <f t="shared" si="2"/>
         <v>1.2789699570815449</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <f t="shared" si="3"/>
         <v>2.8669527896995706</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <f t="shared" si="4"/>
         <v>3.3047210300429186</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>6.11</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>2.66</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>2.58</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>6.22</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>7.37</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <f t="shared" si="0"/>
         <v>0.51779661016949152</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <f t="shared" si="1"/>
         <v>1.1416309012875536</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <f t="shared" si="2"/>
         <v>1.1072961373390557</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <f t="shared" si="3"/>
         <v>2.6695278969957079</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <f t="shared" si="4"/>
         <v>3.1630901287553645</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>7.55</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>2.52</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>2.57</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>5.9</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>6.88</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>5</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <f t="shared" si="0"/>
         <v>0.63983050847457623</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f t="shared" si="1"/>
         <v>1.0815450643776823</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <f t="shared" si="2"/>
         <v>1.1030042918454934</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <f t="shared" si="3"/>
         <v>2.5321888412017168</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <f t="shared" si="4"/>
         <v>2.9527896995708152</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>8.25</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>2.44</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>2.56</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>5.61</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>6.45</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>6</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
         <v>0.69915254237288127</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <f t="shared" si="1"/>
         <v>1.0472103004291844</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <f t="shared" si="2"/>
         <v>1.0987124463519313</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <f t="shared" si="3"/>
         <v>2.407725321888412</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <f t="shared" si="4"/>
         <v>2.7682403433476397</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>9.89</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>5.25</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>6.09</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>7</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <f t="shared" si="0"/>
         <v>0.83813559322033893</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <f t="shared" si="1"/>
         <v>0.98712446351931316</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <f t="shared" si="2"/>
         <v>1.0686695278969958</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <f t="shared" si="3"/>
         <v>2.2532188841201717</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <f t="shared" si="4"/>
         <v>2.6137339055793989</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>10.69</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>2.19</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>2.38</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>5.18</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>5.87</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>8</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <f t="shared" si="0"/>
         <v>0.90593220338983038</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <f t="shared" si="1"/>
         <v>0.93991416309012865</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <f t="shared" si="2"/>
         <v>1.0214592274678111</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <f t="shared" si="3"/>
         <v>2.2231759656652357</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="6">
         <f t="shared" si="4"/>
         <v>2.5193133047210301</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>11.34</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>2.13</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>2.27</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>4.88</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>5.68</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>9</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <f t="shared" si="0"/>
         <v>0.96101694915254232</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <f t="shared" si="1"/>
         <v>0.9141630901287553</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <f t="shared" si="2"/>
         <v>0.97424892703862653</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <f t="shared" si="3"/>
         <v>2.0944206008583688</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <f t="shared" si="4"/>
         <v>2.4377682403433476</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>11.71</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>2.09</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>2.2200000000000002</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>4.82</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>5.6</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>10</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <f t="shared" si="0"/>
         <v>0.99237288135593227</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <f t="shared" si="1"/>
         <v>0.89699570815450635</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <f t="shared" si="2"/>
         <v>0.9527896995708155</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <f t="shared" si="3"/>
         <v>2.0686695278969958</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <f t="shared" si="4"/>
         <v>2.4034334763948495</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="18" spans="2:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="I18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>2.33</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>5.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>5.86</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <f>(C20*1)/$I$3</f>
         <v>0</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <f>(D20*1)/$I$2</f>
         <v>1</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="6">
         <f>(E20*1)/$I$2</f>
         <v>1.0429184549356223</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="6">
         <f>(F20*1)/$I$2</f>
         <v>2.3605150214592272</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="6">
         <f>(G20*1)/$I$2</f>
         <v>2.515021459227468</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>3.1</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>2.83</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>3.02</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>6.7</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>7.88</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>2</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <f t="shared" ref="J21:J26" si="5">(C21*1)/$I$3</f>
         <v>0.26271186440677963</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <f t="shared" ref="K21:K26" si="6">(D21*1)/$I$2</f>
         <v>1.2145922746781115</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <f t="shared" ref="L21:L26" si="7">(E21*1)/$I$2</f>
         <v>1.296137339055794</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="6">
         <f t="shared" ref="M21:M26" si="8">(F21*1)/$I$2</f>
         <v>2.8755364806866952</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N21" s="6">
         <f t="shared" ref="N21:N26" si="9">(G21*1)/$I$2</f>
         <v>3.3819742489270386</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>5.97</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>2.65</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>2.82</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>6.22</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>7.36</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <v>3</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <f t="shared" si="5"/>
         <v>0.50593220338983047</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <f t="shared" si="6"/>
         <v>1.1373390557939913</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="6">
         <f t="shared" si="7"/>
         <v>1.2103004291845492</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="6">
         <f t="shared" si="8"/>
         <v>2.6695278969957079</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="6">
         <f t="shared" si="9"/>
         <v>3.1587982832618025</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>8.32</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>2.5</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>2.7</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>5.65</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>6.56</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>4</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <f t="shared" si="5"/>
         <v>0.70508474576271185</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <f t="shared" si="6"/>
         <v>1.0729613733905579</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="6">
         <f t="shared" si="7"/>
         <v>1.1587982832618027</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="6">
         <f t="shared" si="8"/>
         <v>2.4248927038626609</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="6">
         <f t="shared" si="9"/>
         <v>2.8154506437768236</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>10.18</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>2.2799999999999998</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>2.41</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>5.17</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>5.93</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>5</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="5">
         <f t="shared" si="5"/>
         <v>0.8627118644067796</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <f t="shared" si="6"/>
         <v>0.97854077253218874</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="6">
         <f t="shared" si="7"/>
         <v>1.0343347639484979</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <f t="shared" si="8"/>
         <v>2.2188841201716736</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="6">
         <f t="shared" si="9"/>
         <v>2.5450643776824031</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <v>6</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>11.4</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>2.09</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>2.27</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>4.8499999999999996</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>5.64</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>6</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="5">
         <f t="shared" si="5"/>
         <v>0.96610169491525422</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="6">
         <f t="shared" si="6"/>
         <v>0.89699570815450635</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="6">
         <f t="shared" si="7"/>
         <v>0.97424892703862653</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="6">
         <f t="shared" si="8"/>
         <v>2.0815450643776821</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <f t="shared" si="9"/>
         <v>2.4206008583690983</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
         <v>7</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>11.86</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>2.0099999999999998</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>2.2200000000000002</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>4.75</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>5.51</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>7</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="5">
         <f t="shared" si="5"/>
         <v>1.0050847457627117</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="6">
         <f t="shared" si="6"/>
         <v>0.86266094420600847</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="6">
         <f t="shared" si="7"/>
         <v>0.9527896995708155</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="6">
         <f t="shared" si="8"/>
         <v>2.0386266094420602</v>
       </c>
-      <c r="N26" s="7">
+      <c r="N26" s="6">
         <f t="shared" si="9"/>
         <v>2.3648068669527897</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="D5:G5"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I18:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>